<commit_message>
Add knowledge in ChengYu
</commit_message>
<xml_diff>
--- a/ChengYu/res/knowledge/knowledge.xlsx
+++ b/ChengYu/res/knowledge/knowledge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="关卡" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,9 @@
     <sheet name="成语接龙" sheetId="5" r:id="rId6"/>
     <sheet name="手疾眼快" sheetId="6" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">手疾眼快!$A$1:$B$3</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>关卡回合</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -182,10 +185,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>内容</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一鸣惊人落井下石眼疾手快语无伦次</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -195,6 +194,25 @@
   </si>
   <si>
     <t>黑白颠倒,心血来潮,一夫当关,五颜六色,五彩斑斓,蹑手蹑脚,夸父追日,十全十美</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关卡ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一鸣惊人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十全十美</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>题目</t>
+  </si>
+  <si>
+    <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -254,8 +272,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -274,11 +308,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="21">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -616,136 +666,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>2</v>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>3</v>
       </c>
     </row>
@@ -837,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -869,7 +952,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -903,10 +986,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -933,7 +1016,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="42.75">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -950,7 +1033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="42.75">
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -967,9 +1050,6 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1"/>
-    <row r="5" spans="1:5" s="3" customFormat="1"/>
-    <row r="6" spans="1:5" s="3" customFormat="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -986,7 +1066,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -999,7 +1079,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1007,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1015,12 +1095,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1031,16 +1112,45 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="DG1" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="42.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1051,14 +1161,42 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>